<commit_message>
Updated status and deleted baseball.c
</commit_message>
<xml_diff>
--- a/Neetcode/Neetcode_status.xlsx
+++ b/Neetcode/Neetcode_status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\jigya\Desktop\Github_Projects\DataStructures_and_Algorithms\Neetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D12568-33F8-4931-8E2F-A1A63822A576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FBF73E-F68A-4492-B188-6504DEC9E670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode List" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="326">
   <si>
     <t>Category</t>
   </si>
@@ -999,13 +999,16 @@
   </si>
   <si>
     <t>Create a hashtable with value  as key, in the for loop you check if the value exists(return true) else add the value. Clear the hashtable before leaving</t>
+  </si>
+  <si>
+    <t>Create an array with occurrence of each alphabet stored for both strings, compare the two arrays to check if occurences are different</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1097,8 +1100,15 @@
       <name val="Roboto"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Roboto"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1131,7 +1141,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1193,10 +1209,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1228,9 +1245,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1450,7 +1470,7 @@
   <dimension ref="A1:AA1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1508,7 +1528,7 @@
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>323</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -1547,11 +1567,15 @@
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="25" t="s">
+        <v>323</v>
+      </c>
       <c r="D3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>325</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1583,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="9"/>

</xml_diff>